<commit_message>
simplified event filter creation APIs slightly
git-svn-id: https://www.hpi.uni-potsdam.de/giese/gforge/svn/bp2009/sources/trunk@1458 3ca8e212-6386-4b1e-b09d-39f68028012c
</commit_message>
<xml_diff>
--- a/de.hpi.sam.bp2009.solution.eventManager/measuringInternalTableImprovements.xlsx
+++ b/de.hpi.sam.bp2009.solution.eventManager/measuringInternalTableImprovements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="20940" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="20940" windowHeight="12405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ratio new vs. naive" sheetId="16" r:id="rId1"/>
@@ -242,23 +242,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="132437504"/>
-        <c:axId val="132439040"/>
+        <c:axId val="87680896"/>
+        <c:axId val="99635584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132437504"/>
+        <c:axId val="87680896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132439040"/>
+        <c:crossAx val="99635584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132439040"/>
+        <c:axId val="99635584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -266,7 +266,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132437504"/>
+        <c:crossAx val="87680896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -279,7 +279,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -491,23 +491,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="121861632"/>
-        <c:axId val="121863168"/>
+        <c:axId val="100307328"/>
+        <c:axId val="100308864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121861632"/>
+        <c:axId val="100307328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121863168"/>
+        <c:crossAx val="100308864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121863168"/>
+        <c:axId val="100308864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,20 +515,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121861632"/>
+        <c:crossAx val="100307328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -740,23 +739,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="121935744"/>
-        <c:axId val="121937280"/>
+        <c:axId val="100321152"/>
+        <c:axId val="100322688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121935744"/>
+        <c:axId val="100321152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121937280"/>
+        <c:crossAx val="100322688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121937280"/>
+        <c:axId val="100322688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -764,20 +763,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121935744"/>
+        <c:crossAx val="100321152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -989,23 +987,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="121977088"/>
-        <c:axId val="122007552"/>
+        <c:axId val="100420992"/>
+        <c:axId val="100430976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121977088"/>
+        <c:axId val="100420992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122007552"/>
+        <c:crossAx val="100430976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122007552"/>
+        <c:axId val="100430976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,7 +1011,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121977088"/>
+        <c:crossAx val="100420992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1026,7 +1024,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1238,23 +1236,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="122161792"/>
-        <c:axId val="122175872"/>
+        <c:axId val="100545664"/>
+        <c:axId val="100547200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122161792"/>
+        <c:axId val="100545664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122175872"/>
+        <c:crossAx val="100547200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122175872"/>
+        <c:axId val="100547200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1260,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122161792"/>
+        <c:crossAx val="100545664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1275,7 +1273,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1487,23 +1485,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="122097024"/>
-        <c:axId val="122102912"/>
+        <c:axId val="100563584"/>
+        <c:axId val="100565376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122097024"/>
+        <c:axId val="100563584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122102912"/>
+        <c:crossAx val="100565376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122102912"/>
+        <c:axId val="100565376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1511,7 +1509,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122097024"/>
+        <c:crossAx val="100563584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1524,7 +1522,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1835,23 +1833,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115027968"/>
-        <c:axId val="115029504"/>
+        <c:axId val="100632064"/>
+        <c:axId val="100633600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115027968"/>
+        <c:axId val="100632064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115029504"/>
+        <c:crossAx val="100633600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115029504"/>
+        <c:axId val="100633600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,7 +1857,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115027968"/>
+        <c:crossAx val="100632064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1872,7 +1870,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2183,23 +2181,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115109888"/>
-        <c:axId val="115111424"/>
+        <c:axId val="100470784"/>
+        <c:axId val="100472320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115109888"/>
+        <c:axId val="100470784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115111424"/>
+        <c:crossAx val="100472320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115111424"/>
+        <c:axId val="100472320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2205,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115109888"/>
+        <c:crossAx val="100470784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2220,7 +2218,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2531,23 +2529,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115347456"/>
-        <c:axId val="115348992"/>
+        <c:axId val="100505856"/>
+        <c:axId val="100507648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115347456"/>
+        <c:axId val="100505856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115348992"/>
+        <c:crossAx val="100507648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115348992"/>
+        <c:axId val="100507648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2555,7 +2553,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115347456"/>
+        <c:crossAx val="100505856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2568,7 +2566,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2879,23 +2877,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115417088"/>
-        <c:axId val="115418624"/>
+        <c:axId val="100680448"/>
+        <c:axId val="100681984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115417088"/>
+        <c:axId val="100680448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115418624"/>
+        <c:crossAx val="100681984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115418624"/>
+        <c:axId val="100681984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2903,7 +2901,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115417088"/>
+        <c:crossAx val="100680448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2916,7 +2914,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3227,23 +3225,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115527680"/>
-        <c:axId val="115529216"/>
+        <c:axId val="100711424"/>
+        <c:axId val="100721408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115527680"/>
+        <c:axId val="100711424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115529216"/>
+        <c:crossAx val="100721408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115529216"/>
+        <c:axId val="100721408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,7 +3249,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115527680"/>
+        <c:crossAx val="100711424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3264,7 +3262,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3378,23 +3376,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="124370944"/>
-        <c:axId val="124372480"/>
+        <c:axId val="99650944"/>
+        <c:axId val="99669120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124370944"/>
+        <c:axId val="99650944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124372480"/>
+        <c:crossAx val="99669120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124372480"/>
+        <c:axId val="99669120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3402,7 +3400,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124370944"/>
+        <c:crossAx val="99650944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3415,7 +3413,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3726,23 +3724,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115568640"/>
-        <c:axId val="115570176"/>
+        <c:axId val="100808192"/>
+        <c:axId val="100809728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115568640"/>
+        <c:axId val="100808192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115570176"/>
+        <c:crossAx val="100809728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115570176"/>
+        <c:axId val="100809728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3750,7 +3748,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115568640"/>
+        <c:crossAx val="100808192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3763,7 +3761,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4074,23 +4072,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="9466240"/>
-        <c:axId val="9467776"/>
+        <c:axId val="100859904"/>
+        <c:axId val="100861440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9466240"/>
+        <c:axId val="100859904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9467776"/>
+        <c:crossAx val="100861440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="9467776"/>
+        <c:axId val="100861440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4098,7 +4096,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9466240"/>
+        <c:crossAx val="100859904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4111,7 +4109,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4620,23 +4618,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="9560448"/>
-        <c:axId val="9561984"/>
+        <c:axId val="100929920"/>
+        <c:axId val="100931456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9560448"/>
+        <c:axId val="100929920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9561984"/>
+        <c:crossAx val="100931456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="9561984"/>
+        <c:axId val="100931456"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4645,7 +4643,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="9560448"/>
+        <c:crossAx val="100929920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4658,7 +4656,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5167,23 +5165,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56193408"/>
-        <c:axId val="56194944"/>
+        <c:axId val="100954496"/>
+        <c:axId val="100956032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56193408"/>
+        <c:axId val="100954496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56194944"/>
+        <c:crossAx val="100956032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56194944"/>
+        <c:axId val="100956032"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5192,7 +5190,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56193408"/>
+        <c:crossAx val="100954496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5205,7 +5203,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5714,23 +5712,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115605888"/>
-        <c:axId val="115607424"/>
+        <c:axId val="101065088"/>
+        <c:axId val="101066624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115605888"/>
+        <c:axId val="101065088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115607424"/>
+        <c:crossAx val="101066624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115607424"/>
+        <c:axId val="101066624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5739,7 +5737,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115605888"/>
+        <c:crossAx val="101065088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5752,7 +5750,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6261,23 +6259,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115655040"/>
-        <c:axId val="115656576"/>
+        <c:axId val="101106048"/>
+        <c:axId val="101107584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115655040"/>
+        <c:axId val="101106048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115656576"/>
+        <c:crossAx val="101107584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115656576"/>
+        <c:axId val="101107584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6286,7 +6284,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115655040"/>
+        <c:crossAx val="101106048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6299,7 +6297,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6808,23 +6806,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="53502336"/>
-        <c:axId val="53503872"/>
+        <c:axId val="101159296"/>
+        <c:axId val="101160832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53502336"/>
+        <c:axId val="101159296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53503872"/>
+        <c:crossAx val="101160832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53503872"/>
+        <c:axId val="101160832"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6833,7 +6831,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53502336"/>
+        <c:crossAx val="101159296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6846,7 +6844,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7355,23 +7353,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56250752"/>
-        <c:axId val="56252288"/>
+        <c:axId val="101192064"/>
+        <c:axId val="101193600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56250752"/>
+        <c:axId val="101192064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56252288"/>
+        <c:crossAx val="101193600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56252288"/>
+        <c:axId val="101193600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7380,7 +7378,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56250752"/>
+        <c:crossAx val="101192064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7393,7 +7391,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7902,23 +7900,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56292096"/>
-        <c:axId val="56293632"/>
+        <c:axId val="101237504"/>
+        <c:axId val="101239040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56292096"/>
+        <c:axId val="101237504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56293632"/>
+        <c:crossAx val="101239040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56293632"/>
+        <c:axId val="101239040"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7927,20 +7925,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56292096"/>
+        <c:crossAx val="101237504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8054,23 +8051,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="127523072"/>
-        <c:axId val="127074304"/>
+        <c:axId val="100016512"/>
+        <c:axId val="100018048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127523072"/>
+        <c:axId val="100016512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127074304"/>
+        <c:crossAx val="100018048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127074304"/>
+        <c:axId val="100018048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8078,7 +8075,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127523072"/>
+        <c:crossAx val="100016512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8091,7 +8088,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8205,23 +8202,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="127103744"/>
-        <c:axId val="127105280"/>
+        <c:axId val="100045952"/>
+        <c:axId val="100047488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127103744"/>
+        <c:axId val="100045952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127105280"/>
+        <c:crossAx val="100047488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127105280"/>
+        <c:axId val="100047488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8229,7 +8226,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127103744"/>
+        <c:crossAx val="100045952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8242,7 +8239,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8356,23 +8353,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="127130624"/>
-        <c:axId val="130482944"/>
+        <c:axId val="100079488"/>
+        <c:axId val="100081024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127130624"/>
+        <c:axId val="100079488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130482944"/>
+        <c:crossAx val="100081024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130482944"/>
+        <c:axId val="100081024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8380,7 +8377,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127130624"/>
+        <c:crossAx val="100079488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8393,7 +8390,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8507,23 +8504,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="130528768"/>
-        <c:axId val="130530304"/>
+        <c:axId val="100088448"/>
+        <c:axId val="100118912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130528768"/>
+        <c:axId val="100088448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130530304"/>
+        <c:crossAx val="100118912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130530304"/>
+        <c:axId val="100118912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8531,7 +8528,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130528768"/>
+        <c:crossAx val="100088448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8544,7 +8541,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8658,23 +8655,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="131026944"/>
-        <c:axId val="131028480"/>
+        <c:axId val="100126080"/>
+        <c:axId val="100140160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131026944"/>
+        <c:axId val="100126080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131028480"/>
+        <c:crossAx val="100140160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131028480"/>
+        <c:axId val="100140160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8682,7 +8679,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131026944"/>
+        <c:crossAx val="100126080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8695,7 +8692,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8907,23 +8904,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="121627392"/>
-        <c:axId val="121628928"/>
+        <c:axId val="100353152"/>
+        <c:axId val="100354688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121627392"/>
+        <c:axId val="100353152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121628928"/>
+        <c:crossAx val="100354688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121628928"/>
+        <c:axId val="100354688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8931,7 +8928,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121627392"/>
+        <c:crossAx val="100353152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8944,7 +8941,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9156,23 +9153,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="121758848"/>
-        <c:axId val="121760384"/>
+        <c:axId val="100379264"/>
+        <c:axId val="100393344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121758848"/>
+        <c:axId val="100379264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121760384"/>
+        <c:crossAx val="100393344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121760384"/>
+        <c:axId val="100393344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9180,20 +9177,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121758848"/>
+        <c:crossAx val="100379264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10346,8 +10342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A46" activePane="bottomLeft"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="615" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1:G1048576"/>
       <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
     </sheetView>
@@ -14609,8 +14605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A43" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="615" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1:G1048576"/>
       <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
     </sheetView>

</xml_diff>